<commit_message>
adds MyAccount page,DataProvider clss, LoginData.xlsx and TC_login Test also done with ExcelUtility
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -19,25 +19,25 @@
     <t>Password</t>
   </si>
   <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>OogwayDoe@gmail.com</t>
+  </si>
+  <si>
+    <t>Oogway@123</t>
+  </si>
+  <si>
     <t>Valid</t>
   </si>
   <si>
-    <t>JohnDoe@Gmail.com</t>
-  </si>
-  <si>
-    <t>john@123</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>JeorgeSmith@Gmail.com</t>
   </si>
   <si>
     <t>Jeorge@125</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Invalid</t>
   </si>
   <si>
     <t>Sonu@gmail.com</t>

</xml_diff>